<commit_message>
Add of 3D-unet model training and prediction
</commit_message>
<xml_diff>
--- a/Models/Statistical_analysis.xlsx
+++ b/Models/Statistical_analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Antoine\TN10_uOttawa\codes\PFI_Autosegmentation_project\Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59EE767D-608E-43EC-BEF6-7CA3DFE3903A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA19142-48E4-49C3-8A77-9F0FF14A15A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" xr2:uid="{03D99370-1E69-4C30-882A-F3CC81D1ADBD}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="61">
   <si>
     <t>Model</t>
   </si>
@@ -205,6 +205,21 @@
   </si>
   <si>
     <t>Mpunet_23DATA</t>
+  </si>
+  <si>
+    <t>3Dunet_41DATA_split1</t>
+  </si>
+  <si>
+    <t>3Dunet_41DATA_split2</t>
+  </si>
+  <si>
+    <t>3Dunet_41DATA_split3</t>
+  </si>
+  <si>
+    <t>3Dunet_41DATA_mean</t>
+  </si>
+  <si>
+    <t>3Dunet_41data</t>
   </si>
 </sst>
 </file>
@@ -499,31 +514,12 @@
             </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="4"/>
+            <c:idx val="5"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="00B050"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000000-03BB-4797-954E-98BD554DBEB8}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="5"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -542,6 +538,13 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
+                <c:extLst>
+                  <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                    <c15:fullRef>
+                      <c15:sqref>Models_general_performances!$M$6:$S$6</c15:sqref>
+                    </c15:fullRef>
+                  </c:ext>
+                </c:extLst>
                 <c:f>Models_general_performances!$M$6:$R$6</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
@@ -556,9 +559,12 @@
                     <c:v>4.4271796975133212E-2</c:v>
                   </c:pt>
                   <c:pt idx="3">
+                    <c:v>2.2918406454549942E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
                     <c:v>8.0746449561631944E-3</c:v>
                   </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="5">
                     <c:v>2.8373391330832026E-2</c:v>
                   </c:pt>
                 </c:numCache>
@@ -566,6 +572,13 @@
             </c:plus>
             <c:minus>
               <c:numRef>
+                <c:extLst>
+                  <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                    <c15:fullRef>
+                      <c15:sqref>Models_general_performances!$M$6:$S$6</c15:sqref>
+                    </c15:fullRef>
+                  </c:ext>
+                </c:extLst>
                 <c:f>Models_general_performances!$M$6:$R$6</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
@@ -580,9 +593,12 @@
                     <c:v>4.4271796975133212E-2</c:v>
                   </c:pt>
                   <c:pt idx="3">
+                    <c:v>2.2918406454549942E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
                     <c:v>8.0746449561631944E-3</c:v>
                   </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="5">
                     <c:v>2.8373391330832026E-2</c:v>
                   </c:pt>
                 </c:numCache>
@@ -601,6 +617,13 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Models_general_performances!$M$4:$S$4</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
               <c:f>Models_general_performances!$M$4:$R$4</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
@@ -614,19 +637,26 @@
                   <c:v>Mpunet_35DATA_fusion</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>3Dunet_41data</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>Mpunet_41DATA</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>Mpunet_41DATA_fusion</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Mpunet_43DATA (2 bad data=&gt; 61 &amp; 69)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Models_general_performances!$M$5:$S$5</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
               <c:f>Models_general_performances!$M$5:$R$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -641,18 +671,36 @@
                   <c:v>0.81945333333333326</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>0.71916333333333338</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>0.72929666666666659</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.79457333333333324</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.67993000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:categoryFilterExceptions>
+                <c15:categoryFilterException>
+                  <c15:sqref>Models_general_performances!$S$5</c15:sqref>
+                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c15:spPr>
+                  <c15:invertIfNegative val="0"/>
+                  <c15:bubble3D val="0"/>
+                </c15:categoryFilterException>
+              </c15:categoryFilterExceptions>
+            </c:ext>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-8BD8-4D47-A123-F9A67A6EC555}"/>
             </c:ext>
@@ -695,8 +743,43 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="6"/>
+              <c:pt idx="0">
+                <c:v>Mpunet_23DATA</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Mpunet_35DATA</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>Mpunet_35DATA_fusion</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>3Dunet_41data</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>Mpunet_41DATA</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>Mpunet_41DATA_fusion</c:v>
+              </c:pt>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:autoCat val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:strLit>
+          </c:cat>
           <c:val>
             <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Models_general_performances!$M$7:$S$7</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
               <c:f>Models_general_performances!$M$7:$R$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -750,8 +833,43 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="6"/>
+              <c:pt idx="0">
+                <c:v>Mpunet_23DATA</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Mpunet_35DATA</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>Mpunet_35DATA_fusion</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>3Dunet_41data</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>Mpunet_41DATA</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>Mpunet_41DATA_fusion</c:v>
+              </c:pt>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:autoCat val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:strLit>
+          </c:cat>
           <c:val>
             <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Models_general_performances!$M$8:$S$8</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
               <c:f>Models_general_performances!$M$8:$R$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -1165,7 +1283,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>(Models_general_performances!$M$6,Models_general_performances!$N$6,Models_general_performances!$P$6)</c:f>
+                <c:f>(Models_general_performances!$M$6,Models_general_performances!$N$6,Models_general_performances!$Q$6)</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -1183,7 +1301,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>(Models_general_performances!$M$6,Models_general_performances!$N$6,Models_general_performances!$P$6)</c:f>
+                <c:f>(Models_general_performances!$M$6,Models_general_performances!$N$6,Models_general_performances!$Q$6)</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -1235,7 +1353,7 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>(Models_general_performances!$M$9,Models_general_performances!$N$9,Models_general_performances!$P$9)</c:f>
+              <c:f>(Models_general_performances!$M$9,Models_general_performances!$N$9,Models_general_performances!$Q$9)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1253,7 +1371,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>(Models_general_performances!$M$5,Models_general_performances!$N$5,Models_general_performances!$P$5)</c:f>
+              <c:f>(Models_general_performances!$M$5,Models_general_performances!$N$5,Models_general_performances!$Q$5)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -3865,16 +3983,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>578225</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>159125</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>260725</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>82488</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>314216</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>180897</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>347061</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>104260</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4262,8 +4380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37DEAD19-3658-4779-AADC-1133095E7AE1}">
   <dimension ref="A1:AAP35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="58" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="77" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6455,16 +6573,18 @@
       <c r="O4" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="P4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="R4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="R4" s="2" t="s">
+      <c r="S4" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="S4" s="1"/>
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
       <c r="V4" s="1"/>
@@ -7194,17 +7314,20 @@
         <v>0.81945333333333326</v>
       </c>
       <c r="P5" s="2">
+        <f>D35</f>
+        <v>0.71916333333333338</v>
+      </c>
+      <c r="Q5" s="2">
         <f>D8</f>
         <v>0.72929666666666659</v>
       </c>
-      <c r="Q5" s="2">
+      <c r="R5" s="2">
         <f>D13</f>
         <v>0.79457333333333324</v>
       </c>
-      <c r="R5" s="2">
+      <c r="S5" s="2">
         <v>0.67993000000000003</v>
       </c>
-      <c r="S5" s="1"/>
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
       <c r="V5" s="1"/>
@@ -7934,14 +8057,17 @@
         <v>4.4271796975133212E-2</v>
       </c>
       <c r="P6" s="2">
+        <f>G35</f>
+        <v>2.2918406454549942E-2</v>
+      </c>
+      <c r="Q6" s="2">
         <f>G8</f>
         <v>8.0746449561631944E-3</v>
       </c>
-      <c r="Q6" s="2">
+      <c r="R6" s="2">
         <f>G13</f>
         <v>2.8373391330832026E-2</v>
       </c>
-      <c r="S6" s="1"/>
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
       <c r="V6" s="1"/>
@@ -8675,14 +8801,17 @@
         <v>0.71</v>
       </c>
       <c r="Q7" s="2">
-        <f t="shared" ref="P7:R7" si="0">$C2</f>
+        <f>$C2</f>
         <v>0.71</v>
       </c>
       <c r="R7" s="2">
+        <f t="shared" ref="Q7:S7" si="0">$C2</f>
+        <v>0.71</v>
+      </c>
+      <c r="S7" s="2">
         <f t="shared" si="0"/>
         <v>0.71</v>
       </c>
-      <c r="S7" s="1"/>
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
       <c r="V7" s="1"/>
@@ -9436,14 +9565,17 @@
         <v>0.89</v>
       </c>
       <c r="Q8" s="1">
-        <f t="shared" ref="P8:R8" si="1">$D2</f>
+        <f>$D2</f>
         <v>0.89</v>
       </c>
       <c r="R8" s="1">
+        <f t="shared" ref="Q8:S8" si="1">$D2</f>
+        <v>0.89</v>
+      </c>
+      <c r="S8" s="1">
         <f t="shared" si="1"/>
         <v>0.89</v>
       </c>
-      <c r="S8" s="1"/>
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
       <c r="V8" s="1"/>
@@ -10159,16 +10291,18 @@
       <c r="O9" s="1">
         <v>35</v>
       </c>
-      <c r="P9" s="1">
+      <c r="P9" s="2">
         <v>41</v>
       </c>
       <c r="Q9" s="1">
         <v>41</v>
       </c>
       <c r="R9" s="1">
+        <v>41</v>
+      </c>
+      <c r="S9" s="1">
         <v>43</v>
       </c>
-      <c r="S9" s="1"/>
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
       <c r="V9" s="1"/>
@@ -16013,9 +16147,10 @@
       <c r="A25" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="4">
         <v>35</v>
       </c>
+      <c r="C25" s="4"/>
       <c r="D25" s="4">
         <f>AVERAGE(D22:D24)</f>
         <v>0.81945333333333326</v>
@@ -16116,14 +16251,80 @@
         <v>0.77044409524189861</v>
       </c>
     </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A32" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32" s="2">
+        <v>41</v>
+      </c>
+      <c r="C32" s="2">
+        <v>1</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0.71987999999999996</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A33" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B33" s="2">
+        <v>41</v>
+      </c>
+      <c r="C33" s="2">
+        <v>2</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0.70960000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A34" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" s="2">
+        <v>41</v>
+      </c>
+      <c r="C34" s="2">
+        <v>3</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0.72801000000000005</v>
+      </c>
+    </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
+      <c r="A35" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35" s="4">
+        <v>41</v>
+      </c>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4">
+        <f>AVERAGE(D32:D34)</f>
+        <v>0.71916333333333338</v>
+      </c>
+      <c r="E35" s="4">
+        <f>_xlfn.STDEV.S(D32:D34)</f>
+        <v>9.2259001367527085E-3</v>
+      </c>
+      <c r="F35" s="4">
+        <f>_xlfn.T.INV.2T(0.05,2)</f>
+        <v>4.3026527297494637</v>
+      </c>
+      <c r="G35" s="4">
+        <f>F35*(E35/(3^(1/2)))</f>
+        <v>2.2918406454549942E-2</v>
+      </c>
+      <c r="H35" s="4">
+        <f>D35-G35</f>
+        <v>0.69624492687878348</v>
+      </c>
+      <c r="I35" s="4">
+        <f>D35+G35</f>
+        <v>0.74208173978788328</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Insertion progress and general update
-Advancements in the Insertion script (not functional yet)
-Add surface meshes transformation features
-Updated mean shape morphed once using the ACLC shapes.
</commit_message>
<xml_diff>
--- a/Models/Statistical_analysis.xlsx
+++ b/Models/Statistical_analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Antoine\TN10_uOttawa\codes\PFI_Autosegmentation_project\Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D460EA0-08D4-483A-A9B9-310DA5E5CEB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18BBB220-DA8F-4664-9890-A8D703AD6A2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" xr2:uid="{03D99370-1E69-4C30-882A-F3CC81D1ADBD}"/>
+    <workbookView xWindow="10710" yWindow="0" windowWidth="10980" windowHeight="13770" xr2:uid="{03D99370-1E69-4C30-882A-F3CC81D1ADBD}"/>
   </bookViews>
   <sheets>
     <sheet name="NEW_Models_general_performances" sheetId="3" r:id="rId1"/>
@@ -229,10 +229,10 @@
     <t>OLD_Mpunet_fusion</t>
   </si>
   <si>
-    <t>NEW_Mpunet</t>
+    <t>3Dunet</t>
   </si>
   <si>
-    <t>NEW_Mpunet_fusion</t>
+    <t>Mpunet</t>
   </si>
 </sst>
 </file>
@@ -539,6 +539,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-D61E-4231-BC23-43FB6084D8E8}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:errBars>
             <c:errBarType val="both"/>
@@ -606,13 +611,13 @@
                   <c:v>OLD_Mpunet</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>NEW_Mpunet</c:v>
+                  <c:v>3Dunet</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>OLD_Mpunet_fusion</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>NEW_Mpunet_fusion</c:v>
+                  <c:v>Mpunet</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1030,6 +1035,697 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR" b="1" u="sng"/>
+              <a:t>Mean general</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-FR" b="1" u="sng" baseline="0"/>
+              <a:t> dice score for different models (Error with student's law </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="el-GR" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>α</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-FR" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>=0.05)</a:t>
+            </a:r>
+            <a:endParaRPr lang="fr-FR" b="1" u="sng"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.3221763261216019E-2"/>
+          <c:y val="8.7694756276444491E-2"/>
+          <c:w val="0.92322963545172765"/>
+          <c:h val="0.85764493493587235"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-46CA-4B22-B996-26E0C370C5F9}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:extLst>
+                  <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                    <c15:fullRef>
+                      <c15:sqref>NEW_Models_general_performances!$M$6:$P$6</c15:sqref>
+                    </c15:fullRef>
+                  </c:ext>
+                </c:extLst>
+                <c:f>(NEW_Models_general_performances!$N$6,NEW_Models_general_performances!$P$6)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>1.9665021573959083E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2.9310172324798711E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:extLst>
+                  <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                    <c15:fullRef>
+                      <c15:sqref>NEW_Models_general_performances!$M$6:$P$6</c15:sqref>
+                    </c15:fullRef>
+                  </c:ext>
+                </c:extLst>
+                <c:f>(NEW_Models_general_performances!$N$6,NEW_Models_general_performances!$P$6)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>1.9665021573959083E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2.9310172324798711E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:srgbClr val="C00000"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>NEW_Models_general_performances!$M$4:$S$4</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(NEW_Models_general_performances!$N$4,NEW_Models_general_performances!$P$4:$S$4)</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>3Dunet</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mpunet</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>NEW_Models_general_performances!$M$5:$P$5</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(NEW_Models_general_performances!$N$5,NEW_Models_general_performances!$P$5)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.7921999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.85404999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:categoryFilterExceptions>
+                <c15:categoryFilterException>
+                  <c15:sqref>NEW_Models_general_performances!$O$5</c15:sqref>
+                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <a:solidFill>
+                      <a:srgbClr val="00B050"/>
+                    </a:solidFill>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c15:spPr>
+                  <c15:invertIfNegative val="0"/>
+                  <c15:bubble3D val="0"/>
+                </c15:categoryFilterException>
+              </c15:categoryFilterExceptions>
+            </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-46CA-4B22-B996-26E0C370C5F9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1873913679"/>
+        <c:axId val="1873914159"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Mpunet publications</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="2"/>
+              <c:pt idx="0">
+                <c:v>3Dunet</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Mpunet</c:v>
+              </c:pt>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:autoCat val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>NEW_Models_general_performances!$M$7:$P$7</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(NEW_Models_general_performances!$N$7,NEW_Models_general_performances!$P$7)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.71</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.71</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-46CA-4B22-B996-26E0C370C5F9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Reference MAX</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="2"/>
+              <c:pt idx="0">
+                <c:v>3Dunet</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Mpunet</c:v>
+              </c:pt>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:autoCat val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>NEW_Models_general_performances!$M$8:$P$8</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(NEW_Models_general_performances!$N$8,NEW_Models_general_performances!$P$8)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.89</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.89</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-46CA-4B22-B996-26E0C370C5F9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1873913679"/>
+        <c:axId val="1873914159"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1873913679"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1873914159"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1873914159"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0.60000000000000009"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>General</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fr-FR" baseline="0"/>
+                  <a:t> dice score</a:t>
+                </a:r>
+                <a:endParaRPr lang="fr-FR"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1873913679"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:legendEntry>
+        <c:idx val="0"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="2"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.0449459883694897E-2"/>
+          <c:y val="1.910323821027432E-2"/>
+          <c:w val="0.12444469631687764"/>
+          <c:h val="3.9899147204458883E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -1814,7 +2510,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -2332,7 +3028,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -3063,6 +3759,46 @@
 </file>
 
 <file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -4109,6 +4845,509 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4624,7 +5863,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5132,15 +6371,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>399738</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>36301</xdr:rowOff>
+      <xdr:colOff>283106</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>23342</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>51999</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>146266</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>2216184</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>133307</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5162,6 +6401,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>64796</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Graphique 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0AEADA62-BD0B-4B25-A20E-892413217062}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5607,8 +6884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE6BDF23-7073-4F0B-AEB5-F0C6A9578DBE}">
   <dimension ref="A1:AAP35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="49" zoomScaleNormal="49" workbookViewId="0">
-      <selection activeCell="M51" sqref="M51"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9992,7 +11269,7 @@
         <v>0.71</v>
       </c>
       <c r="P7" s="2">
-        <f t="shared" ref="N7:S7" si="0">$C2</f>
+        <f t="shared" ref="P7" si="0">$C2</f>
         <v>0.71</v>
       </c>
       <c r="T7" s="1"/>
@@ -10742,7 +12019,7 @@
         <v>0.89</v>
       </c>
       <c r="P8" s="1">
-        <f t="shared" ref="N8:S8" si="1">$D2</f>
+        <f t="shared" ref="P8" si="1">$D2</f>
         <v>0.89</v>
       </c>
       <c r="S8" s="1"/>
@@ -14363,10 +15640,22 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
+      <c r="M13" s="2">
+        <f>M5-M6</f>
+        <v>0.72122202171050342</v>
+      </c>
+      <c r="N13" s="2">
+        <f t="shared" ref="N13:P13" si="2">N5-N6</f>
+        <v>0.7725349784260408</v>
+      </c>
+      <c r="O13" s="2">
+        <f t="shared" si="2"/>
+        <v>0.76619994200250119</v>
+      </c>
+      <c r="P13" s="2">
+        <f t="shared" si="2"/>
+        <v>0.82473982767520126</v>
+      </c>
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
@@ -15071,6 +16360,22 @@
       <c r="AAP13" s="1"/>
     </row>
     <row r="14" spans="1:718" x14ac:dyDescent="0.35">
+      <c r="M14" s="2">
+        <f>M5+M6</f>
+        <v>0.73737131162282976</v>
+      </c>
+      <c r="N14" s="2">
+        <f t="shared" ref="N14:P14" si="3">N5+N6</f>
+        <v>0.81186502157395901</v>
+      </c>
+      <c r="O14" s="2">
+        <f t="shared" si="3"/>
+        <v>0.8229467246641653</v>
+      </c>
+      <c r="P14" s="2">
+        <f t="shared" si="3"/>
+        <v>0.88336017232479869</v>
+      </c>
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>

</xml_diff>